<commit_message>
Finished Sprint 1 Backlog and Burndown Chart
</commit_message>
<xml_diff>
--- a/Burndown Chart.xlsx
+++ b/Burndown Chart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewlam/Documents/csce315/CSCE-315-Project2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documents\csce315\CSCE-315-Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Project 2 Group 4</t>
   </si>
@@ -195,12 +195,21 @@
   </si>
   <si>
     <t xml:space="preserve">total hours </t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>hours left</t>
+  </si>
+  <si>
+    <t>sprint progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -244,12 +253,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -288,7 +300,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -321,8 +332,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
@@ -339,16 +350,28 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:spPr>
@@ -390,7 +413,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -409,49 +431,197 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$D$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$D$55:$G$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>86.0</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D327-4FF5-85B3-73FA5B31C135}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Sprint 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-D327-4FF5-85B3-73FA5B31C135}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="t"/>
@@ -462,11 +632,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="820142464"/>
         <c:axId val="814080592"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="820142464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -499,7 +668,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -529,7 +697,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -568,12 +736,8 @@
         </c:txPr>
         <c:crossAx val="814080592"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="0"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="814080592"/>
         <c:scaling>
@@ -621,7 +785,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -651,6 +814,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -695,7 +859,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1335,7 +1498,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1616,28 +1785,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection sqref="A1:D54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.8125" customWidth="1"/>
+    <col min="2" max="2" width="16.1875" customWidth="1"/>
     <col min="3" max="3" width="47" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.1875" customWidth="1"/>
+    <col min="5" max="5" width="14.1875" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B1" s="1"/>
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="D2">
         <v>0</v>
       </c>
@@ -1650,8 +1823,26 @@
       <c r="G2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0.25</v>
+      </c>
+      <c r="L2">
+        <v>0.5</v>
+      </c>
+      <c r="M2">
+        <v>0.75</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1673,8 +1864,26 @@
       <c r="G3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3">
+        <v>86</v>
+      </c>
+      <c r="K3">
+        <v>80</v>
+      </c>
+      <c r="L3">
+        <v>76</v>
+      </c>
+      <c r="M3">
+        <v>68</v>
+      </c>
+      <c r="N3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1682,7 +1891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B5">
         <v>1.1000000000000001</v>
       </c>
@@ -1702,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B6">
         <v>1.2</v>
       </c>
@@ -1722,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B7">
         <v>1.3</v>
       </c>
@@ -1742,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B8">
         <v>1.4</v>
       </c>
@@ -1762,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B9">
         <v>1.5</v>
       </c>
@@ -1782,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B10">
         <v>1.6</v>
       </c>
@@ -1802,7 +2011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B11">
         <v>1.7</v>
       </c>
@@ -1822,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B12">
         <v>1.8</v>
       </c>
@@ -1842,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B13">
         <v>1.9</v>
       </c>
@@ -1862,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B14" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -1882,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B15">
         <v>1.1100000000000001</v>
       </c>
@@ -1902,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B16">
         <v>1.1200000000000001</v>
       </c>
@@ -1922,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B17">
         <v>1.1299999999999999</v>
       </c>
@@ -1942,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B18">
         <v>1.1399999999999999</v>
       </c>
@@ -1962,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B19">
         <v>1.1499999999999999</v>
       </c>
@@ -1982,17 +2191,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B22">
         <v>2.1</v>
       </c>
@@ -2012,7 +2221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B23">
         <v>2.2000000000000002</v>
       </c>
@@ -2032,7 +2241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B24">
         <v>2.2999999999999998</v>
       </c>
@@ -2052,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B25">
         <v>2.4</v>
       </c>
@@ -2072,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B26">
         <v>2.5</v>
       </c>
@@ -2092,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B27">
         <v>2.6</v>
       </c>
@@ -2112,7 +2321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B28">
         <v>2.7</v>
       </c>
@@ -2132,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B29">
         <v>2.8</v>
       </c>
@@ -2152,7 +2361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B30">
         <v>2.9</v>
       </c>
@@ -2172,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B31" s="2">
         <v>2.1</v>
       </c>
@@ -2192,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B32">
         <v>2.11</v>
       </c>
@@ -2212,7 +2421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2220,7 +2429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B35">
         <v>3.1</v>
       </c>
@@ -2240,7 +2449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B36">
         <v>3.2</v>
       </c>
@@ -2260,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B37">
         <v>3.3</v>
       </c>
@@ -2280,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B38">
         <v>3.4</v>
       </c>
@@ -2300,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B39">
         <v>3.5</v>
       </c>
@@ -2320,7 +2529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B40">
         <v>3.6</v>
       </c>
@@ -2340,7 +2549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B41">
         <v>3.7</v>
       </c>
@@ -2360,7 +2569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B42">
         <v>3.8</v>
       </c>
@@ -2380,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2388,7 +2597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B45">
         <v>4.0999999999999996</v>
       </c>
@@ -2408,7 +2617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B46">
         <v>4.2</v>
       </c>
@@ -2428,7 +2637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B47">
         <v>4.3</v>
       </c>
@@ -2448,7 +2657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B48">
         <v>4.3</v>
       </c>
@@ -2468,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B49">
         <v>4.4000000000000004</v>
       </c>
@@ -2488,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B50">
         <v>4.5</v>
       </c>
@@ -2508,7 +2717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B51">
         <v>4.5999999999999996</v>
       </c>
@@ -2528,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B52">
         <v>4.7</v>
       </c>
@@ -2548,7 +2757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.5">
       <c r="C54" t="s">
         <v>55</v>
       </c>
@@ -2568,7 +2777,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.5">
       <c r="C55" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
Sprint 1 Retrospective and Sprint 2 backlogs
</commit_message>
<xml_diff>
--- a/Burndown Chart.xlsx
+++ b/Burndown Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documents\csce315\CSCE-315-Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documents\csce315\CSCE-315-Project2-local\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Project 2 Group 4</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>sprint progress</t>
+  </si>
+  <si>
+    <t>client acknowledgement</t>
+  </si>
+  <si>
+    <t>allow random distribution of seeds</t>
+  </si>
+  <si>
+    <t>implement "pie rule"</t>
   </si>
 </sst>
 </file>
@@ -340,7 +349,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$55</c:f>
+              <c:f>Sheet1!$C$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -454,15 +463,15 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$55:$G$55</c:f>
+              <c:f>Sheet1!$D$58:$G$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>26</c:v>
@@ -599,19 +608,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>76</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1486,15 +1495,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>608012</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>735012</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>15876</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1785,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:N3"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1868,19 +1877,19 @@
         <v>57</v>
       </c>
       <c r="J3">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K3">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L3">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M3">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="N3">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.5">
@@ -2165,10 +2174,10 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.5">
@@ -2185,77 +2194,75 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A20" t="s">
-        <v>21</v>
+      <c r="B20">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B22">
-        <v>2.1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22">
-        <v>4</v>
-      </c>
-      <c r="E22">
-        <v>4</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
+        <v>1.17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
       <c r="B23">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B24">
-        <v>2.2999999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -2263,19 +2270,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B25">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D25">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E25">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -2283,19 +2290,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B26">
-        <v>2.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -2303,39 +2310,39 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B27">
-        <v>2.6</v>
+        <v>2.4</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27">
         <v>5</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
       <c r="F27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B28">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -2343,30 +2350,30 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B29">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B30">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -2382,20 +2389,20 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B31" s="2">
-        <v>2.1</v>
+      <c r="B31">
+        <v>2.8</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -2403,87 +2410,87 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B32">
+        <v>2.9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B33" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B34">
         <v>2.11</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
         <v>32</v>
       </c>
-      <c r="D32">
+      <c r="D34">
         <v>3</v>
       </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A34" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B36">
         <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B35">
-        <v>3.1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35">
-        <v>2</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>2</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B36">
-        <v>3.2</v>
-      </c>
-      <c r="C36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B37">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2491,10 +2498,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B38">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -2503,18 +2510,18 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B39">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -2531,30 +2538,30 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B40">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B41">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2571,81 +2578,81 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B42">
+        <v>3.6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B43">
+        <v>3.7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B44">
         <v>3.8</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>41</v>
       </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A44" t="s">
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A46" t="s">
         <v>42</v>
       </c>
-      <c r="B44">
+      <c r="B46">
         <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B45">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C45" t="s">
-        <v>43</v>
-      </c>
-      <c r="D45">
-        <v>3</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B46">
-        <v>4.2</v>
-      </c>
-      <c r="C46" t="s">
-        <v>44</v>
-      </c>
-      <c r="D46">
-        <v>2</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B47">
-        <v>4.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C47" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -2654,18 +2661,18 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B48">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2674,18 +2681,18 @@
         <v>0</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B49">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -2694,18 +2701,18 @@
         <v>0</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B50">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2714,15 +2721,15 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B51">
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -2739,60 +2746,120 @@
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B52">
+        <v>4.5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B53">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C53" t="s">
+        <v>49</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B54">
         <v>4.7</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>50</v>
       </c>
-      <c r="D52">
+      <c r="D54">
         <v>3</v>
       </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.5">
-      <c r="C54" t="s">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B55">
+        <v>4.8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="C57" t="s">
         <v>55</v>
       </c>
-      <c r="D54">
-        <f>SUM(D5:D19,D22:D32,D35:D42,D45:D52)</f>
-        <v>86</v>
-      </c>
-      <c r="E54">
-        <f>SUM(E5:E19,E22:E32)</f>
+      <c r="D57">
+        <v>89</v>
+      </c>
+      <c r="E57">
+        <f>SUM(E5:E19,E24:E34)</f>
         <v>30</v>
       </c>
-      <c r="F54">
-        <f>SUM(F5:F19,F22:F32,F35:F42,F45:F52)</f>
-        <v>30</v>
-      </c>
-      <c r="G54">
+      <c r="F57">
+        <f>SUM(F5:F21,F24:F34,F37:F44,F47:F55)</f>
+        <v>33</v>
+      </c>
+      <c r="G57">
+        <f>SUM(G5:G21,G24:G34,G37:G44,G47:G55)</f>
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.5">
-      <c r="C55" t="s">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="C58" t="s">
         <v>51</v>
       </c>
-      <c r="D55">
-        <v>86</v>
-      </c>
-      <c r="E55">
-        <f>86-30</f>
-        <v>56</v>
-      </c>
-      <c r="F55">
-        <f>E55-F54</f>
+      <c r="D58">
+        <v>89</v>
+      </c>
+      <c r="E58">
+        <f>D58-E57</f>
+        <v>59</v>
+      </c>
+      <c r="F58">
+        <f>E58-F57</f>
         <v>26</v>
       </c>
-      <c r="G55">
+      <c r="G58">
         <v>0</v>
       </c>
     </row>

</xml_diff>